<commit_message>
CTMS - Structure creation. [Pages, Steps]
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/StudyManagement/StudyManagementTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/StudyManagement/StudyManagementTestData.xlsx
@@ -33,9 +33,6 @@
     <t>User</t>
   </si>
   <si>
-    <t>AddStudy</t>
-  </si>
-  <si>
     <t>Study Phase</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>Planning</t>
+  </si>
+  <si>
+    <t>AddNewStudy</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -386,7 +386,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -400,7 +400,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -409,10 +409,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -423,10 +423,10 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">

</xml_diff>